<commit_message>
Fix update nhân viên
</commit_message>
<xml_diff>
--- a/admin/pages/User-Based/result/1_original_matrix.xlsx
+++ b/admin/pages/User-Based/result/1_original_matrix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CW39"/>
+  <dimension ref="A1:CW40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1905,14 +1905,20 @@
       <c r="BG9" t="inlineStr"/>
       <c r="BH9" t="inlineStr"/>
       <c r="BI9" t="inlineStr"/>
-      <c r="BJ9" t="inlineStr"/>
-      <c r="BK9" t="inlineStr"/>
+      <c r="BJ9" t="n">
+        <v>8</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>8</v>
+      </c>
       <c r="BL9" t="inlineStr"/>
       <c r="BM9" t="n">
         <v>28</v>
       </c>
       <c r="BN9" t="inlineStr"/>
-      <c r="BO9" t="inlineStr"/>
+      <c r="BO9" t="n">
+        <v>8</v>
+      </c>
       <c r="BP9" t="inlineStr"/>
       <c r="BQ9" t="inlineStr"/>
       <c r="BR9" t="inlineStr"/>
@@ -4957,7 +4963,7 @@
         <v>16</v>
       </c>
       <c r="C35" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
@@ -5070,12 +5076,10 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" t="inlineStr"/>
-      <c r="C36" t="n">
-        <v>18</v>
-      </c>
+      <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
@@ -5099,7 +5103,9 @@
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="inlineStr"/>
-      <c r="AA36" t="inlineStr"/>
+      <c r="AA36" t="n">
+        <v>14</v>
+      </c>
       <c r="AB36" t="inlineStr"/>
       <c r="AC36" t="inlineStr"/>
       <c r="AD36" t="inlineStr"/>
@@ -5177,12 +5183,12 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>64</v>
-      </c>
-      <c r="B37" t="n">
-        <v>24</v>
-      </c>
-      <c r="C37" t="inlineStr"/>
+        <v>63</v>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="n">
+        <v>18</v>
+      </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
@@ -5206,9 +5212,7 @@
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="inlineStr"/>
-      <c r="AA37" t="n">
-        <v>10</v>
-      </c>
+      <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr"/>
       <c r="AC37" t="inlineStr"/>
       <c r="AD37" t="inlineStr"/>
@@ -5286,10 +5290,10 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" t="n">
-        <v>2946</v>
+        <v>24</v>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
@@ -5301,9 +5305,7 @@
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
-      <c r="M38" t="n">
-        <v>7</v>
-      </c>
+      <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
@@ -5317,11 +5319,11 @@
       <c r="X38" t="inlineStr"/>
       <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="inlineStr"/>
-      <c r="AA38" t="inlineStr"/>
+      <c r="AA38" t="n">
+        <v>10</v>
+      </c>
       <c r="AB38" t="inlineStr"/>
-      <c r="AC38" t="n">
-        <v>176</v>
-      </c>
+      <c r="AC38" t="inlineStr"/>
       <c r="AD38" t="inlineStr"/>
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr"/>
@@ -5343,9 +5345,7 @@
       <c r="AV38" t="inlineStr"/>
       <c r="AW38" t="inlineStr"/>
       <c r="AX38" t="inlineStr"/>
-      <c r="AY38" t="n">
-        <v>8</v>
-      </c>
+      <c r="AY38" t="inlineStr"/>
       <c r="AZ38" t="inlineStr"/>
       <c r="BA38" t="inlineStr"/>
       <c r="BB38" t="inlineStr"/>
@@ -5378,9 +5378,7 @@
       <c r="CC38" t="inlineStr"/>
       <c r="CD38" t="inlineStr"/>
       <c r="CE38" t="inlineStr"/>
-      <c r="CF38" t="n">
-        <v>25</v>
-      </c>
+      <c r="CF38" t="inlineStr"/>
       <c r="CG38" t="inlineStr"/>
       <c r="CH38" t="inlineStr"/>
       <c r="CI38" t="inlineStr"/>
@@ -5401,10 +5399,10 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B39" t="n">
-        <v>16</v>
+        <v>2946</v>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
@@ -5416,7 +5414,9 @@
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr"/>
+      <c r="M39" t="n">
+        <v>7</v>
+      </c>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
@@ -5432,7 +5432,9 @@
       <c r="Z39" t="inlineStr"/>
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr"/>
-      <c r="AC39" t="inlineStr"/>
+      <c r="AC39" t="n">
+        <v>176</v>
+      </c>
       <c r="AD39" t="inlineStr"/>
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr"/>
@@ -5454,15 +5456,15 @@
       <c r="AV39" t="inlineStr"/>
       <c r="AW39" t="inlineStr"/>
       <c r="AX39" t="inlineStr"/>
-      <c r="AY39" t="inlineStr"/>
+      <c r="AY39" t="n">
+        <v>8</v>
+      </c>
       <c r="AZ39" t="inlineStr"/>
       <c r="BA39" t="inlineStr"/>
       <c r="BB39" t="inlineStr"/>
       <c r="BC39" t="inlineStr"/>
       <c r="BD39" t="inlineStr"/>
-      <c r="BE39" t="n">
-        <v>8</v>
-      </c>
+      <c r="BE39" t="inlineStr"/>
       <c r="BF39" t="inlineStr"/>
       <c r="BG39" t="inlineStr"/>
       <c r="BH39" t="inlineStr"/>
@@ -5489,7 +5491,9 @@
       <c r="CC39" t="inlineStr"/>
       <c r="CD39" t="inlineStr"/>
       <c r="CE39" t="inlineStr"/>
-      <c r="CF39" t="inlineStr"/>
+      <c r="CF39" t="n">
+        <v>25</v>
+      </c>
       <c r="CG39" t="inlineStr"/>
       <c r="CH39" t="inlineStr"/>
       <c r="CI39" t="inlineStr"/>
@@ -5508,6 +5512,115 @@
       <c r="CV39" t="inlineStr"/>
       <c r="CW39" t="inlineStr"/>
     </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>67</v>
+      </c>
+      <c r="B40" t="n">
+        <v>16</v>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+      <c r="X40" t="inlineStr"/>
+      <c r="Y40" t="inlineStr"/>
+      <c r="Z40" t="inlineStr"/>
+      <c r="AA40" t="inlineStr"/>
+      <c r="AB40" t="inlineStr"/>
+      <c r="AC40" t="inlineStr"/>
+      <c r="AD40" t="inlineStr"/>
+      <c r="AE40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr"/>
+      <c r="AG40" t="inlineStr"/>
+      <c r="AH40" t="inlineStr"/>
+      <c r="AI40" t="inlineStr"/>
+      <c r="AJ40" t="inlineStr"/>
+      <c r="AK40" t="inlineStr"/>
+      <c r="AL40" t="inlineStr"/>
+      <c r="AM40" t="inlineStr"/>
+      <c r="AN40" t="inlineStr"/>
+      <c r="AO40" t="inlineStr"/>
+      <c r="AP40" t="inlineStr"/>
+      <c r="AQ40" t="inlineStr"/>
+      <c r="AR40" t="inlineStr"/>
+      <c r="AS40" t="inlineStr"/>
+      <c r="AT40" t="inlineStr"/>
+      <c r="AU40" t="inlineStr"/>
+      <c r="AV40" t="inlineStr"/>
+      <c r="AW40" t="inlineStr"/>
+      <c r="AX40" t="inlineStr"/>
+      <c r="AY40" t="inlineStr"/>
+      <c r="AZ40" t="inlineStr"/>
+      <c r="BA40" t="inlineStr"/>
+      <c r="BB40" t="inlineStr"/>
+      <c r="BC40" t="inlineStr"/>
+      <c r="BD40" t="inlineStr"/>
+      <c r="BE40" t="n">
+        <v>8</v>
+      </c>
+      <c r="BF40" t="inlineStr"/>
+      <c r="BG40" t="inlineStr"/>
+      <c r="BH40" t="inlineStr"/>
+      <c r="BI40" t="inlineStr"/>
+      <c r="BJ40" t="inlineStr"/>
+      <c r="BK40" t="inlineStr"/>
+      <c r="BL40" t="inlineStr"/>
+      <c r="BM40" t="inlineStr"/>
+      <c r="BN40" t="inlineStr"/>
+      <c r="BO40" t="inlineStr"/>
+      <c r="BP40" t="inlineStr"/>
+      <c r="BQ40" t="inlineStr"/>
+      <c r="BR40" t="inlineStr"/>
+      <c r="BS40" t="inlineStr"/>
+      <c r="BT40" t="inlineStr"/>
+      <c r="BU40" t="inlineStr"/>
+      <c r="BV40" t="inlineStr"/>
+      <c r="BW40" t="inlineStr"/>
+      <c r="BX40" t="inlineStr"/>
+      <c r="BY40" t="inlineStr"/>
+      <c r="BZ40" t="inlineStr"/>
+      <c r="CA40" t="inlineStr"/>
+      <c r="CB40" t="inlineStr"/>
+      <c r="CC40" t="inlineStr"/>
+      <c r="CD40" t="inlineStr"/>
+      <c r="CE40" t="inlineStr"/>
+      <c r="CF40" t="inlineStr"/>
+      <c r="CG40" t="inlineStr"/>
+      <c r="CH40" t="inlineStr"/>
+      <c r="CI40" t="inlineStr"/>
+      <c r="CJ40" t="inlineStr"/>
+      <c r="CK40" t="inlineStr"/>
+      <c r="CL40" t="inlineStr"/>
+      <c r="CM40" t="inlineStr"/>
+      <c r="CN40" t="inlineStr"/>
+      <c r="CO40" t="inlineStr"/>
+      <c r="CP40" t="inlineStr"/>
+      <c r="CQ40" t="inlineStr"/>
+      <c r="CR40" t="inlineStr"/>
+      <c r="CS40" t="inlineStr"/>
+      <c r="CT40" t="inlineStr"/>
+      <c r="CU40" t="inlineStr"/>
+      <c r="CV40" t="inlineStr"/>
+      <c r="CW40" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>